<commit_message>
Change use of Google API to OpenStreetMap
</commit_message>
<xml_diff>
--- a/document.xlsx
+++ b/document.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\arent-film-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\arent-sf-movie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5E18A8-3387-4019-AEBA-AFFE4D81E443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA9325-B116-4EC9-B3D6-97CB745047E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="4" r:id="rId1"/>
     <sheet name="FrontEnd" sheetId="1" r:id="rId2"/>
     <sheet name="BackEnd" sheetId="2" r:id="rId3"/>
     <sheet name="GG Map API" sheetId="3" r:id="rId4"/>
+    <sheet name="OpenStreetMap" sheetId="5" r:id="rId5"/>
+    <sheet name="QGIS 3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Flask</t>
   </si>
@@ -64,6 +66,18 @@
   </si>
   <si>
     <t>https://wiki.matbao.net/kb/huong-dan-khoi-tao-google-maps-api-de-chen-vao-website/</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/925164/openstreetmap-embedding-map-in-webpage-like-google-maps</t>
+  </si>
+  <si>
+    <t>https://qgis.org/en/docs/index.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjzorWent35AhVflFYBHWpMBdUQFnoECAwQAQ&amp;url=https%3A%2F%2Ftowardsdatascience.com%2Floading-data-from-openstreetmap-with-python-and-the-overpass-api-513882a27fd0&amp;usg=AOvVaw3YLvFD8iUT1pcjWWphxab4</t>
+  </si>
+  <si>
+    <t>https://pygis.io/docs/d_access_osm.html</t>
   </si>
 </sst>
 </file>
@@ -489,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59711EE9-DAB2-44F2-B135-B518C840A6C5}">
   <dimension ref="B2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -518,4 +532,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C30B8-C29F-4D45-A11C-A54271649D6E}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{39266AD0-3524-4795-8991-96C7CD33C9D8}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjzorWent35AhVflFYBHWpMBdUQFnoECAwQAQ&amp;url=https%3A%2F%2Ftowardsdatascience.com%2Floading-data-from-openstreetmap-with-python-and-the-overpass-api-513882a27fd0&amp;usg=AOvVaw3YLvFD8iUT1pcjWWphxab4" xr:uid="{9D2D3BC7-2FB7-4A62-89EB-4E837465E257}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{166BCA2F-0657-46B1-BC49-6382DFA616D3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F67294-392A-4113-9C1C-3C9FB0333DED}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B98962BA-DDCC-4A3C-83A6-1344CFFB2E34}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add .ipynb file; preprocessing address for querying
</commit_message>
<xml_diff>
--- a/document.xlsx
+++ b/document.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\arent-sf-movie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Project\arent-sf-movie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA9325-B116-4EC9-B3D6-97CB745047E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1C070C-5E8B-47E6-A8CD-ABBD5914F13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="4" r:id="rId1"/>
-    <sheet name="FrontEnd" sheetId="1" r:id="rId2"/>
-    <sheet name="BackEnd" sheetId="2" r:id="rId3"/>
-    <sheet name="GG Map API" sheetId="3" r:id="rId4"/>
-    <sheet name="OpenStreetMap" sheetId="5" r:id="rId5"/>
-    <sheet name="QGIS 3" sheetId="6" r:id="rId6"/>
+    <sheet name="Workflows" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId3"/>
+    <sheet name="FrontEnd" sheetId="1" r:id="rId4"/>
+    <sheet name="BackEnd" sheetId="2" r:id="rId5"/>
+    <sheet name="GG Map API" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="OpenStreetMap" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Flask</t>
   </si>
@@ -71,13 +72,114 @@
     <t>https://stackoverflow.com/questions/925164/openstreetmap-embedding-map-in-webpage-like-google-maps</t>
   </si>
   <si>
-    <t>https://qgis.org/en/docs/index.html</t>
-  </si>
-  <si>
     <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjzorWent35AhVflFYBHWpMBdUQFnoECAwQAQ&amp;url=https%3A%2F%2Ftowardsdatascience.com%2Floading-data-from-openstreetmap-with-python-and-the-overpass-api-513882a27fd0&amp;usg=AOvVaw3YLvFD8iUT1pcjWWphxab4</t>
   </si>
   <si>
     <t>https://pygis.io/docs/d_access_osm.html</t>
+  </si>
+  <si>
+    <t>https://nominatim.org/release-docs/develop/api/Search/</t>
+  </si>
+  <si>
+    <t>Đọc file CSV để lấy lịch sử phim đã được chiếu</t>
+  </si>
+  <si>
+    <t>Hiển thị bản đồ San Francisco tổng quan</t>
+  </si>
+  <si>
+    <t>Hiện thị toàn bộ marker các địa điểm chiếu phim</t>
+  </si>
+  <si>
+    <t>_ and _ Street</t>
+  </si>
+  <si>
+    <t>Tiền xử lí dữ liệu "địa chỉ" (Locations) sao cho thành chuỗi truy vấn dùng cho url</t>
+  </si>
+  <si>
+    <t>20th and Folsom Streets</t>
+  </si>
+  <si>
+    <t>street=Folsom+%26+20th</t>
+  </si>
+  <si>
+    <t>https://nominatim.openstreetmap.org/search.php?street=Folsom+%26+20th&amp;city=san+francisco&amp;format=jsonv2</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "place_id": 68854055,
+        "licence": "Data © OpenStreetMap contributors, ODbL 1.0. https://osm.org/copyright",
+        "osm_type": "node",
+        "osm_id": 6384663492,
+        "boundingbox": [
+            "37.758673",
+            "37.758773",
+            "-122.4148487",
+            "-122.4147487"
+        ],
+        "lat": "37.758723",
+        "lon": "-122.4147987",
+        "display_name": "Folsom Street &amp; 20th Street, Folsom Street, Mission District, San Francisco, California, 90103, United States",
+        "place_rank": 30,
+        "category": "highway",
+        "type": "bus_stop",
+        "importance": 0.4001,
+        "icon": "https://nominatim.openstreetmap.org/ui/mapicons/transport_bus_stop2.p.20.png"
+    }
+]</t>
+  </si>
+  <si>
+    <t>https://nominatim.openstreetmap.org/search.php?q=Golden+Gate+Park%2C+San+Francisco&amp;format=jsonv2</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "place_id": 142363953,
+        "licence": "Data © OpenStreetMap contributors, ODbL 1.0. https://osm.org/copyright",
+        "osm_type": "way",
+        "osm_id": 158602261,
+        "boundingbox": [
+            "37.764142",
+            "37.7746518",
+            "-122.5108673",
+            "-122.45318"
+        ],
+        "lat": "37.769368099999994",
+        "lon": "-122.48218371117709",
+        "display_name": "Golden Gate Park, San Francisco, California, United States",
+        "place_rank": 24,
+        "category": "leisure",
+        "type": "park",
+        "importance": 0.955740352341206
+    }
+]</t>
+  </si>
+  <si>
+    <t>https://thewebdev.info/2022/04/03/how-to-pass-variables-from-python-flask-to-javascript/#:~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template.</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;head&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;script type="text/javascript" {{ url_for('static', filename='app.js')}}&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;script type="text/javascript"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            myVar = myFunc({{ data | tojson }})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;/head&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -120,9 +222,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,19 +513,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -437,6 +540,144 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F01D922-8FC1-480D-B18F-7A804CA30C66}">
+  <dimension ref="B2:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{399757AF-407B-41A9-ACCA-B44C63AE428A}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{C8EDDD16-6638-4A6B-B663-DCEFDC9F16A4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7C06A-2B81-4BE6-831B-C972D84CE522}">
+  <dimension ref="B2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location=":~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template." display="https://thewebdev.info/2022/04/03/how-to-pass-variables-from-python-flask-to-javascript/#:~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template." xr:uid="{D27EEBDE-9BB0-4377-822B-EAEAADE74299}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B7"/>
   <sheetViews>
@@ -444,34 +685,34 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -487,19 +728,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D711C204-F059-4699-97B8-CE5B7DA44B1A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59711EE9-DAB2-44F2-B135-B518C840A6C5}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -507,19 +748,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -534,29 +775,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C30B8-C29F-4D45-A11C-A54271649D6E}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -564,29 +810,7 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{39266AD0-3524-4795-8991-96C7CD33C9D8}"/>
     <hyperlink ref="B4" r:id="rId2" display="https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjzorWent35AhVflFYBHWpMBdUQFnoECAwQAQ&amp;url=https%3A%2F%2Ftowardsdatascience.com%2Floading-data-from-openstreetmap-with-python-and-the-overpass-api-513882a27fd0&amp;usg=AOvVaw3YLvFD8iUT1pcjWWphxab4" xr:uid="{9D2D3BC7-2FB7-4A62-89EB-4E837465E257}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{166BCA2F-0657-46B1-BC49-6382DFA616D3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F67294-392A-4113-9C1C-3C9FB0333DED}">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B98962BA-DDCC-4A3C-83A6-1344CFFB2E34}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{9CECFA35-4448-438C-975B-138F7C72F670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Need to implement autocomplete search input and show markers on map
</commit_message>
<xml_diff>
--- a/document.xlsx
+++ b/document.xlsx
@@ -8,49 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Project\arent-sf-movie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C5047-D4F0-476B-B55A-CAEB520E460E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE14E19F-05A9-4E4E-BB0E-7ED81A8F5538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spent Time" sheetId="9" r:id="rId1"/>
     <sheet name="Requirements" sheetId="4" r:id="rId2"/>
     <sheet name="Workflows" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
-    <sheet name="FrontEnd" sheetId="1" r:id="rId5"/>
-    <sheet name="BackEnd" sheetId="2" r:id="rId6"/>
-    <sheet name="GG Map API" sheetId="3" state="hidden" r:id="rId7"/>
-    <sheet name="OpenStreetMap" sheetId="5" r:id="rId8"/>
+    <sheet name="AutoComplete Search" sheetId="10" r:id="rId4"/>
+    <sheet name="GG Map API" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="OpenStreetMap" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Flask</t>
-  </si>
-  <si>
-    <t>https://flask.palletsprojects.com/en/2.2.x/#</t>
-  </si>
-  <si>
-    <t>Werkzeg WSGI toolkit</t>
-  </si>
-  <si>
-    <t>https://werkzeug.palletsprojects.com/</t>
-  </si>
-  <si>
-    <t>Jinja2 template engine</t>
-  </si>
-  <si>
-    <t>https://jinja.palletsprojects.com/en/3.1.x/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>https://developers.google.com/maps/documentation/javascript/overview</t>
   </si>
@@ -156,31 +144,13 @@
 ]</t>
   </si>
   <si>
-    <t>https://thewebdev.info/2022/04/03/how-to-pass-variables-from-python-flask-to-javascript/#:~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template.</t>
-  </si>
-  <si>
-    <t>&lt;html&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;head&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         &lt;script type="text/javascript" {{ url_for('static', filename='app.js')}}&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         &lt;script type="text/javascript"&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            myVar = myFunc({{ data | tojson }})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         &lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;/head&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/html&gt;</t>
+    <t>https://bootstrap-autocomplete.readthedocs.io/en/latest/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/how-to-create-dynamic-autocomplete-search-using-bootstrap-typeahead/</t>
+  </si>
+  <si>
+    <t>How to create dynamic autocomplete search using Bootstrap Typeahead ?</t>
   </si>
 </sst>
 </file>
@@ -509,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EA4B37-2AD9-4188-B80B-111FA5DC308E}">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -542,6 +512,15 @@
       </c>
       <c r="B4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>44802</v>
+      </c>
+      <c r="B5">
+        <f>0.5</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -561,17 +540,17 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -595,57 +574,57 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -658,133 +637,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7C06A-2B81-4BE6-831B-C972D84CE522}">
-  <dimension ref="B2:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895511F6-B568-4B4D-9B7A-CD998F55AD7C}">
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location=":~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template." display="https://thewebdev.info/2022/04/03/how-to-pass-variables-from-python-flask-to-javascript/#:~:text=To%20pass%20variables%20from%20Python%20Flask%20to%20JavaScript%2C%20we%20can,to%20pass%20to%20the%20template.&amp;text=to%20call%20render_template%20with%20the,to%20pass%20to%20the%20template." xr:uid="{D27EEBDE-9BB0-4377-822B-EAEAADE74299}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{1BB63A93-F40F-47F0-95CE-DD3A4D7B56C9}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{BC598377-A75D-40A2-9FD0-99BCB6401470}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{8424651F-A832-4FD9-96AF-FF3EC67DDD61}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{420424F7-2F57-4B44-93A4-0E0188E6A213}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{30E632ED-2887-4937-BC78-90F77E462390}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D711C204-F059-4699-97B8-CE5B7DA44B1A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59711EE9-DAB2-44F2-B135-B518C840A6C5}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -796,17 +682,17 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C30B8-C29F-4D45-A11C-A54271649D6E}">
   <dimension ref="B2:B7"/>
   <sheetViews>
@@ -831,22 +717,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add spent time to README.md
</commit_message>
<xml_diff>
--- a/document.xlsx
+++ b/document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Project\arent-sf-movie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40976950-75D3-4436-8F16-128D9425028D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0A768A-832D-4D6C-BC76-D9F11113E8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>https://developers.google.com/maps/documentation/javascript/overview</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>How to create dynamic autocomplete search using Bootstrap Typeahead ?</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
 </sst>
 </file>
@@ -478,64 +481,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EA4B37-2AD9-4188-B80B-111FA5DC308E}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2">
         <v>44797</v>
       </c>
-      <c r="B2">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
         <v>44798</v>
       </c>
-      <c r="B3">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
         <v>44799</v>
       </c>
-      <c r="B4">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
         <v>44802</v>
       </c>
-      <c r="B5">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
         <f>0.5</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
         <v>44805</v>
       </c>
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
         <v>44806</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>